<commit_message>
Calculate n_respondents for all variables and add special candidate cases
- Modified calculate_demovote_errors() to calculate n_respondents for ALL variables (demographics, voting,
state), not just election variables
  - Changed n_respondents from NA_integer_ to sum(!is.na(ces_state[[demo_var]])) in three locations (lines
516, 540, 585)
  - Provides consistent tracking across all variable types

- Added special cases in get_top_candidate() for races where top candidate not in CES:
  - 2016 Louisiana U.S. Senate: Select FOSTER CAMPBELL (John Kennedy not listed in CES)
  - 2018 North Dakota Secretary of State: Select Joshua A. Boschee (Al Jaeger dropped out and ran as
independent)
</commit_message>
<xml_diff>
--- a/data/Benchmarks/Election Returns/Senate_0622_clean_fixed.xlsx
+++ b/data/Benchmarks/Election Returns/Senate_0622_clean_fixed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdpruett/Desktop/CES Accuracy Analysis/data/Election Validation/Final Sets - Clean Fixed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdpruett/Desktop/CES Accuracy Analysis/data/Benchmarks/Election Returns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC27A5B6-8234-4A44-B914-1693FB57A8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ADB48A-C982-A845-BBA7-851C5EF4E8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="20280" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13854" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13854" uniqueCount="1354">
   <si>
     <t>year</t>
   </si>
@@ -3196,9 +3196,6 @@
     <t>BAKARI, KAMAU A.</t>
   </si>
   <si>
-    <t>HUGIN, BOB</t>
-  </si>
-  <si>
     <t>HOFFMAN, MADELYN R.</t>
   </si>
   <si>
@@ -4079,6 +4076,12 @@
   </si>
   <si>
     <t>https://elections.wi.gov/elections/election-results#accordion-5604</t>
+  </si>
+  <si>
+    <t>HUGIN, ROBERT</t>
+  </si>
+  <si>
+    <t>MENENDEZ, BOB</t>
   </si>
 </sst>
 </file>
@@ -4433,8 +4436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="I306" sqref="I306"/>
+    <sheetView tabSelected="1" topLeftCell="A1159" workbookViewId="0">
+      <selection activeCell="I1169" sqref="I1169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -60957,7 +60960,7 @@
         <v>0</v>
       </c>
       <c r="I1172" t="s">
-        <v>156</v>
+        <v>1353</v>
       </c>
       <c r="J1172" t="s">
         <v>23</v>
@@ -61007,7 +61010,7 @@
         <v>0</v>
       </c>
       <c r="I1173" t="s">
-        <v>1058</v>
+        <v>1352</v>
       </c>
       <c r="J1173" t="s">
         <v>30</v>
@@ -61057,7 +61060,7 @@
         <v>0</v>
       </c>
       <c r="I1174" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J1174" t="s">
         <v>43</v>
@@ -61104,7 +61107,7 @@
         <v>0</v>
       </c>
       <c r="I1175" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="J1175" t="s">
         <v>33</v>
@@ -61151,10 +61154,10 @@
         <v>0</v>
       </c>
       <c r="I1176" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J1176" t="s">
         <v>1061</v>
-      </c>
-      <c r="J1176" t="s">
-        <v>1062</v>
       </c>
       <c r="K1176" t="b">
         <v>0</v>
@@ -61198,10 +61201,10 @@
         <v>0</v>
       </c>
       <c r="I1177" t="s">
+        <v>1062</v>
+      </c>
+      <c r="J1177" t="s">
         <v>1063</v>
-      </c>
-      <c r="J1177" t="s">
-        <v>1064</v>
       </c>
       <c r="K1177" t="b">
         <v>0</v>
@@ -61245,10 +61248,10 @@
         <v>0</v>
       </c>
       <c r="I1178" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J1178" t="s">
         <v>1065</v>
-      </c>
-      <c r="J1178" t="s">
-        <v>1066</v>
       </c>
       <c r="K1178" t="b">
         <v>0</v>
@@ -61339,7 +61342,7 @@
         <v>0</v>
       </c>
       <c r="I1180" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="J1180" t="s">
         <v>23</v>
@@ -61389,7 +61392,7 @@
         <v>0</v>
       </c>
       <c r="I1181" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="J1181" t="s">
         <v>33</v>
@@ -61439,7 +61442,7 @@
         <v>0</v>
       </c>
       <c r="I1182" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="J1182" t="s">
         <v>30</v>
@@ -61539,7 +61542,7 @@
         <v>0</v>
       </c>
       <c r="I1184" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="J1184" t="s">
         <v>30</v>
@@ -61589,7 +61592,7 @@
         <v>0</v>
       </c>
       <c r="I1185" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="J1185" t="s">
         <v>184</v>
@@ -61777,7 +61780,7 @@
         <v>0</v>
       </c>
       <c r="I1189" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="J1189" t="s">
         <v>349</v>
@@ -61824,7 +61827,7 @@
         <v>0</v>
       </c>
       <c r="I1190" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="J1190" t="s">
         <v>30</v>
@@ -61877,7 +61880,7 @@
         <v>712</v>
       </c>
       <c r="J1191" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="K1191" t="b">
         <v>0</v>
@@ -62068,7 +62071,7 @@
         <v>0</v>
       </c>
       <c r="I1195" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J1195" t="s">
         <v>30</v>
@@ -62168,7 +62171,7 @@
         <v>0</v>
       </c>
       <c r="I1197" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="J1197" t="s">
         <v>30</v>
@@ -62218,7 +62221,7 @@
         <v>0</v>
       </c>
       <c r="I1198" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="J1198" t="s">
         <v>43</v>
@@ -62265,7 +62268,7 @@
         <v>0</v>
       </c>
       <c r="I1199" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="J1199" t="s">
         <v>33</v>
@@ -62365,7 +62368,7 @@
         <v>0</v>
       </c>
       <c r="I1201" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="J1201" t="s">
         <v>30</v>
@@ -62462,7 +62465,7 @@
         <v>0</v>
       </c>
       <c r="I1203" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="J1203" t="s">
         <v>30</v>
@@ -62512,7 +62515,7 @@
         <v>0</v>
       </c>
       <c r="I1204" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="J1204" t="s">
         <v>23</v>
@@ -62562,7 +62565,7 @@
         <v>0</v>
       </c>
       <c r="I1205" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="J1205" t="s">
         <v>40</v>
@@ -62609,7 +62612,7 @@
         <v>0</v>
       </c>
       <c r="I1206" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="J1206" t="s">
         <v>40</v>
@@ -62656,7 +62659,7 @@
         <v>0</v>
       </c>
       <c r="I1207" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="J1207" t="s">
         <v>40</v>
@@ -62703,7 +62706,7 @@
         <v>0</v>
       </c>
       <c r="I1208" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="J1208" t="s">
         <v>40</v>
@@ -62750,7 +62753,7 @@
         <v>0</v>
       </c>
       <c r="I1209" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="J1209" t="s">
         <v>40</v>
@@ -62797,7 +62800,7 @@
         <v>0</v>
       </c>
       <c r="I1210" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="J1210" t="s">
         <v>40</v>
@@ -62894,7 +62897,7 @@
         <v>0</v>
       </c>
       <c r="I1212" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="J1212" t="s">
         <v>23</v>
@@ -62944,7 +62947,7 @@
         <v>0</v>
       </c>
       <c r="I1213" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="J1213" t="s">
         <v>33</v>
@@ -62991,7 +62994,7 @@
         <v>0</v>
       </c>
       <c r="I1214" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="J1214" t="s">
         <v>30</v>
@@ -63041,7 +63044,7 @@
         <v>0</v>
       </c>
       <c r="I1215" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="J1215" t="s">
         <v>23</v>
@@ -63091,7 +63094,7 @@
         <v>0</v>
       </c>
       <c r="I1216" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="J1216" t="s">
         <v>112</v>
@@ -63138,7 +63141,7 @@
         <v>0</v>
       </c>
       <c r="I1217" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="J1217" t="s">
         <v>33</v>
@@ -63188,7 +63191,7 @@
         <v>0</v>
       </c>
       <c r="I1218" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="J1218" t="s">
         <v>565</v>
@@ -63235,7 +63238,7 @@
         <v>0</v>
       </c>
       <c r="I1219" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="J1219" t="s">
         <v>40</v>
@@ -63282,7 +63285,7 @@
         <v>0</v>
       </c>
       <c r="I1220" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="J1220" t="s">
         <v>40</v>
@@ -63329,7 +63332,7 @@
         <v>0</v>
       </c>
       <c r="I1221" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="J1221" t="s">
         <v>40</v>
@@ -63376,7 +63379,7 @@
         <v>0</v>
       </c>
       <c r="I1222" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="J1222" t="s">
         <v>40</v>
@@ -63423,7 +63426,7 @@
         <v>0</v>
       </c>
       <c r="I1223" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="J1223" t="s">
         <v>244</v>
@@ -63470,7 +63473,7 @@
         <v>0</v>
       </c>
       <c r="I1224" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="J1224" t="s">
         <v>40</v>
@@ -63517,7 +63520,7 @@
         <v>0</v>
       </c>
       <c r="I1225" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="J1225" t="s">
         <v>40</v>
@@ -63567,7 +63570,7 @@
         <v>0</v>
       </c>
       <c r="I1226" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="J1226" t="s">
         <v>40</v>
@@ -63614,7 +63617,7 @@
         <v>0</v>
       </c>
       <c r="I1227" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="J1227" t="s">
         <v>30</v>
@@ -63711,7 +63714,7 @@
         <v>0</v>
       </c>
       <c r="I1229" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="J1229" t="s">
         <v>30</v>
@@ -63811,7 +63814,7 @@
         <v>0</v>
       </c>
       <c r="I1231" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="J1231" t="s">
         <v>33</v>
@@ -63958,7 +63961,7 @@
         <v>0</v>
       </c>
       <c r="I1234" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="J1234" t="s">
         <v>30</v>
@@ -64008,7 +64011,7 @@
         <v>0</v>
       </c>
       <c r="I1235" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J1235" t="s">
         <v>23</v>
@@ -64058,7 +64061,7 @@
         <v>0</v>
       </c>
       <c r="I1236" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="J1236" t="s">
         <v>30</v>
@@ -64108,7 +64111,7 @@
         <v>0</v>
       </c>
       <c r="I1237" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="J1237" t="s">
         <v>33</v>
@@ -64205,7 +64208,7 @@
         <v>0</v>
       </c>
       <c r="I1239" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="J1239" t="s">
         <v>30</v>
@@ -64352,7 +64355,7 @@
         <v>0</v>
       </c>
       <c r="I1242" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="J1242" t="s">
         <v>23</v>
@@ -64402,7 +64405,7 @@
         <v>0</v>
       </c>
       <c r="I1243" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J1243" t="s">
         <v>33</v>
@@ -64496,7 +64499,7 @@
         <v>0</v>
       </c>
       <c r="I1245" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J1245" t="s">
         <v>23</v>
@@ -64546,7 +64549,7 @@
         <v>0</v>
       </c>
       <c r="I1246" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="J1246" t="s">
         <v>30</v>
@@ -64643,7 +64646,7 @@
         <v>0</v>
       </c>
       <c r="I1248" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="J1248" t="s">
         <v>40</v>
@@ -64667,7 +64670,7 @@
         <v>293</v>
       </c>
       <c r="Q1248" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="1249" spans="1:16" x14ac:dyDescent="0.2">
@@ -64696,10 +64699,10 @@
         <v>0</v>
       </c>
       <c r="I1249" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J1249" t="s">
         <v>1115</v>
-      </c>
-      <c r="J1249" t="s">
-        <v>1116</v>
       </c>
       <c r="K1249" t="b">
         <v>0</v>
@@ -64840,7 +64843,7 @@
         <v>1</v>
       </c>
       <c r="I1252" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="J1252" t="s">
         <v>945</v>
@@ -64937,7 +64940,7 @@
         <v>1</v>
       </c>
       <c r="I1254" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="J1254" t="s">
         <v>945</v>
@@ -64984,7 +64987,7 @@
         <v>1</v>
       </c>
       <c r="I1255" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="J1255" t="s">
         <v>945</v>
@@ -65031,7 +65034,7 @@
         <v>1</v>
       </c>
       <c r="I1256" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="J1256" t="s">
         <v>945</v>
@@ -65078,7 +65081,7 @@
         <v>1</v>
       </c>
       <c r="I1257" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="J1257" t="s">
         <v>949</v>
@@ -65125,7 +65128,7 @@
         <v>1</v>
       </c>
       <c r="I1258" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="J1258" t="s">
         <v>949</v>
@@ -65172,7 +65175,7 @@
         <v>1</v>
       </c>
       <c r="I1259" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="J1259" t="s">
         <v>949</v>
@@ -65219,7 +65222,7 @@
         <v>1</v>
       </c>
       <c r="I1260" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="J1260" t="s">
         <v>23</v>
@@ -65269,7 +65272,7 @@
         <v>1</v>
       </c>
       <c r="I1261" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="J1261" t="s">
         <v>949</v>
@@ -65316,7 +65319,7 @@
         <v>1</v>
       </c>
       <c r="I1262" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="J1262" t="s">
         <v>33</v>
@@ -65363,7 +65366,7 @@
         <v>1</v>
       </c>
       <c r="I1263" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="J1263" t="s">
         <v>40</v>
@@ -65410,7 +65413,7 @@
         <v>1</v>
       </c>
       <c r="I1264" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="J1264" t="s">
         <v>40</v>
@@ -65457,10 +65460,10 @@
         <v>1</v>
       </c>
       <c r="I1265" t="s">
+        <v>1128</v>
+      </c>
+      <c r="J1265" t="s">
         <v>1129</v>
-      </c>
-      <c r="J1265" t="s">
-        <v>1130</v>
       </c>
       <c r="K1265" t="b">
         <v>1</v>
@@ -65504,7 +65507,7 @@
         <v>1</v>
       </c>
       <c r="I1266" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="J1266" t="s">
         <v>40</v>
@@ -65551,7 +65554,7 @@
         <v>1</v>
       </c>
       <c r="I1267" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="J1267" t="s">
         <v>40</v>
@@ -65598,10 +65601,10 @@
         <v>1</v>
       </c>
       <c r="I1268" t="s">
+        <v>1132</v>
+      </c>
+      <c r="J1268" t="s">
         <v>1133</v>
-      </c>
-      <c r="J1268" t="s">
-        <v>1134</v>
       </c>
       <c r="K1268" t="b">
         <v>1</v>
@@ -65645,7 +65648,7 @@
         <v>1</v>
       </c>
       <c r="I1269" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="J1269" t="s">
         <v>40</v>
@@ -65692,10 +65695,10 @@
         <v>1</v>
       </c>
       <c r="I1270" t="s">
+        <v>1135</v>
+      </c>
+      <c r="J1270" t="s">
         <v>1136</v>
-      </c>
-      <c r="J1270" t="s">
-        <v>1137</v>
       </c>
       <c r="K1270" t="b">
         <v>1</v>
@@ -65739,7 +65742,7 @@
         <v>0</v>
       </c>
       <c r="I1271" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="J1271" t="s">
         <v>33</v>
@@ -65839,7 +65842,7 @@
         <v>0</v>
       </c>
       <c r="I1273" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="J1273" t="s">
         <v>23</v>
@@ -65939,10 +65942,10 @@
         <v>0</v>
       </c>
       <c r="I1275" t="s">
+        <v>1139</v>
+      </c>
+      <c r="J1275" t="s">
         <v>1140</v>
-      </c>
-      <c r="J1275" t="s">
-        <v>1141</v>
       </c>
       <c r="K1275" t="b">
         <v>0</v>
@@ -65986,10 +65989,10 @@
         <v>0</v>
       </c>
       <c r="I1276" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="J1276" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="K1276" t="b">
         <v>0</v>
@@ -66033,7 +66036,7 @@
         <v>0</v>
       </c>
       <c r="I1277" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="J1277" t="s">
         <v>33</v>
@@ -66080,7 +66083,7 @@
         <v>0</v>
       </c>
       <c r="I1278" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="J1278" t="s">
         <v>477</v>
@@ -66127,7 +66130,7 @@
         <v>0</v>
       </c>
       <c r="I1279" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="J1279" t="s">
         <v>43</v>
@@ -66174,7 +66177,7 @@
         <v>0</v>
       </c>
       <c r="I1280" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="J1280" t="s">
         <v>477</v>
@@ -66271,7 +66274,7 @@
         <v>0</v>
       </c>
       <c r="I1282" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="J1282" t="s">
         <v>30</v>
@@ -66321,7 +66324,7 @@
         <v>0</v>
       </c>
       <c r="I1283" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J1283" t="s">
         <v>489</v>
@@ -66465,7 +66468,7 @@
         <v>0</v>
       </c>
       <c r="I1286" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J1286" t="s">
         <v>23</v>
@@ -66515,7 +66518,7 @@
         <v>0</v>
       </c>
       <c r="I1287" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="J1287" t="s">
         <v>33</v>
@@ -66562,7 +66565,7 @@
         <v>0</v>
       </c>
       <c r="I1288" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="J1288" t="s">
         <v>40</v>
@@ -66609,7 +66612,7 @@
         <v>0</v>
       </c>
       <c r="I1289" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J1289" t="s">
         <v>23</v>
@@ -66712,7 +66715,7 @@
         <v>916</v>
       </c>
       <c r="J1291" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="K1291" t="b">
         <v>0</v>
@@ -66806,7 +66809,7 @@
         <v>0</v>
       </c>
       <c r="I1293" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="J1293" t="s">
         <v>30</v>
@@ -66856,10 +66859,10 @@
         <v>0</v>
       </c>
       <c r="I1294" t="s">
+        <v>1154</v>
+      </c>
+      <c r="J1294" t="s">
         <v>1155</v>
-      </c>
-      <c r="J1294" t="s">
-        <v>1156</v>
       </c>
       <c r="K1294" t="b">
         <v>0</v>
@@ -66903,7 +66906,7 @@
         <v>0</v>
       </c>
       <c r="I1295" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="J1295" t="s">
         <v>33</v>
@@ -66950,7 +66953,7 @@
         <v>0</v>
       </c>
       <c r="I1296" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="J1296" t="s">
         <v>43</v>
@@ -66997,7 +67000,7 @@
         <v>0</v>
       </c>
       <c r="I1297" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="J1297" t="s">
         <v>27</v>
@@ -67044,7 +67047,7 @@
         <v>0</v>
       </c>
       <c r="I1298" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="J1298" t="s">
         <v>27</v>
@@ -67091,7 +67094,7 @@
         <v>0</v>
       </c>
       <c r="I1299" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="J1299" t="s">
         <v>27</v>
@@ -67188,7 +67191,7 @@
         <v>0</v>
       </c>
       <c r="I1301" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="J1301" t="s">
         <v>23</v>
@@ -67285,7 +67288,7 @@
         <v>0</v>
       </c>
       <c r="I1303" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="J1303" t="s">
         <v>27</v>
@@ -67379,7 +67382,7 @@
         <v>0</v>
       </c>
       <c r="I1305" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="J1305" t="s">
         <v>30</v>
@@ -67429,7 +67432,7 @@
         <v>0</v>
       </c>
       <c r="I1306" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="J1306" t="s">
         <v>23</v>
@@ -67479,7 +67482,7 @@
         <v>0</v>
       </c>
       <c r="I1307" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="J1307" t="s">
         <v>33</v>
@@ -67576,7 +67579,7 @@
         <v>0</v>
       </c>
       <c r="I1309" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="J1309" t="s">
         <v>23</v>
@@ -67626,7 +67629,7 @@
         <v>0</v>
       </c>
       <c r="I1310" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="J1310" t="s">
         <v>33</v>
@@ -67673,7 +67676,7 @@
         <v>0</v>
       </c>
       <c r="I1311" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="J1311" t="s">
         <v>27</v>
@@ -67720,7 +67723,7 @@
         <v>0</v>
       </c>
       <c r="I1312" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="J1312" t="s">
         <v>27</v>
@@ -67767,7 +67770,7 @@
         <v>0</v>
       </c>
       <c r="I1313" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="J1313" t="s">
         <v>27</v>
@@ -67814,7 +67817,7 @@
         <v>0</v>
       </c>
       <c r="I1314" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="J1314" t="s">
         <v>27</v>
@@ -67861,7 +67864,7 @@
         <v>0</v>
       </c>
       <c r="I1315" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="J1315" t="s">
         <v>27</v>
@@ -67955,7 +67958,7 @@
         <v>0</v>
       </c>
       <c r="I1317" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="J1317" t="s">
         <v>477</v>
@@ -68052,7 +68055,7 @@
         <v>0</v>
       </c>
       <c r="I1319" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="J1319" t="s">
         <v>477</v>
@@ -68146,7 +68149,7 @@
         <v>0</v>
       </c>
       <c r="I1321" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="J1321" t="s">
         <v>28</v>
@@ -68193,7 +68196,7 @@
         <v>0</v>
       </c>
       <c r="I1322" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="J1322" t="s">
         <v>799</v>
@@ -68287,7 +68290,7 @@
         <v>0</v>
       </c>
       <c r="I1324" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="J1324" t="s">
         <v>477</v>
@@ -68334,7 +68337,7 @@
         <v>0</v>
       </c>
       <c r="I1325" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="J1325" t="s">
         <v>804</v>
@@ -68381,7 +68384,7 @@
         <v>0</v>
       </c>
       <c r="I1326" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="J1326" t="s">
         <v>23</v>
@@ -68431,7 +68434,7 @@
         <v>0</v>
       </c>
       <c r="I1327" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J1327" t="s">
         <v>799</v>
@@ -68478,7 +68481,7 @@
         <v>0</v>
       </c>
       <c r="I1328" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="J1328" t="s">
         <v>28</v>
@@ -68525,7 +68528,7 @@
         <v>0</v>
       </c>
       <c r="I1329" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="J1329" t="s">
         <v>33</v>
@@ -68572,7 +68575,7 @@
         <v>0</v>
       </c>
       <c r="I1330" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J1330" t="s">
         <v>799</v>
@@ -68619,7 +68622,7 @@
         <v>0</v>
       </c>
       <c r="I1331" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="J1331" t="s">
         <v>30</v>
@@ -68669,7 +68672,7 @@
         <v>0</v>
       </c>
       <c r="I1332" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="J1332" t="s">
         <v>23</v>
@@ -68719,7 +68722,7 @@
         <v>0</v>
       </c>
       <c r="I1333" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="J1333" t="s">
         <v>40</v>
@@ -68766,7 +68769,7 @@
         <v>0</v>
       </c>
       <c r="I1334" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="J1334" t="s">
         <v>40</v>
@@ -68910,7 +68913,7 @@
         <v>0</v>
       </c>
       <c r="I1337" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="J1337" t="s">
         <v>30</v>
@@ -69054,7 +69057,7 @@
         <v>0</v>
       </c>
       <c r="I1340" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="J1340" t="s">
         <v>23</v>
@@ -69154,7 +69157,7 @@
         <v>0</v>
       </c>
       <c r="I1342" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="J1342" t="s">
         <v>1035</v>
@@ -69295,7 +69298,7 @@
         <v>0</v>
       </c>
       <c r="I1345" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="J1345" t="s">
         <v>27</v>
@@ -69342,7 +69345,7 @@
         <v>0</v>
       </c>
       <c r="I1346" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="J1346" t="s">
         <v>27</v>
@@ -69389,7 +69392,7 @@
         <v>0</v>
       </c>
       <c r="I1347" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="J1347" t="s">
         <v>1040</v>
@@ -69436,10 +69439,10 @@
         <v>0</v>
       </c>
       <c r="I1348" t="s">
+        <v>1194</v>
+      </c>
+      <c r="J1348" t="s">
         <v>1195</v>
-      </c>
-      <c r="J1348" t="s">
-        <v>1196</v>
       </c>
       <c r="K1348" t="b">
         <v>0</v>
@@ -69483,7 +69486,7 @@
         <v>0</v>
       </c>
       <c r="I1349" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="J1349" t="s">
         <v>30</v>
@@ -69533,7 +69536,7 @@
         <v>0</v>
       </c>
       <c r="I1350" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="J1350" t="s">
         <v>23</v>
@@ -69630,7 +69633,7 @@
         <v>0</v>
       </c>
       <c r="I1352" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="J1352" t="s">
         <v>23</v>
@@ -69680,7 +69683,7 @@
         <v>0</v>
       </c>
       <c r="I1353" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="J1353" t="s">
         <v>30</v>
@@ -69730,7 +69733,7 @@
         <v>0</v>
       </c>
       <c r="I1354" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="J1354" t="s">
         <v>33</v>
@@ -69777,7 +69780,7 @@
         <v>0</v>
       </c>
       <c r="I1355" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J1355" t="s">
         <v>23</v>
@@ -69927,7 +69930,7 @@
         <v>0</v>
       </c>
       <c r="I1358" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="J1358" t="s">
         <v>23</v>
@@ -69977,7 +69980,7 @@
         <v>0</v>
       </c>
       <c r="I1359" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="J1359" t="s">
         <v>33</v>
@@ -70024,7 +70027,7 @@
         <v>0</v>
       </c>
       <c r="I1360" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="J1360" t="s">
         <v>27</v>
@@ -70118,7 +70121,7 @@
         <v>0</v>
       </c>
       <c r="I1362" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="J1362" t="s">
         <v>30</v>
@@ -70218,7 +70221,7 @@
         <v>0</v>
       </c>
       <c r="I1364" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="J1364" t="s">
         <v>33</v>
@@ -70312,7 +70315,7 @@
         <v>0</v>
       </c>
       <c r="I1366" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="J1366" t="s">
         <v>23</v>
@@ -70362,7 +70365,7 @@
         <v>0</v>
       </c>
       <c r="I1367" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="J1367" t="s">
         <v>30</v>
@@ -70412,7 +70415,7 @@
         <v>0</v>
       </c>
       <c r="I1368" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="J1368" t="s">
         <v>43</v>
@@ -70459,10 +70462,10 @@
         <v>0</v>
       </c>
       <c r="I1369" t="s">
+        <v>1209</v>
+      </c>
+      <c r="J1369" t="s">
         <v>1210</v>
-      </c>
-      <c r="J1369" t="s">
-        <v>1211</v>
       </c>
       <c r="K1369" t="b">
         <v>0</v>
@@ -70506,10 +70509,10 @@
         <v>0</v>
       </c>
       <c r="I1370" t="s">
+        <v>1211</v>
+      </c>
+      <c r="J1370" t="s">
         <v>1212</v>
-      </c>
-      <c r="J1370" t="s">
-        <v>1213</v>
       </c>
       <c r="K1370" t="b">
         <v>0</v>
@@ -70553,7 +70556,7 @@
         <v>0</v>
       </c>
       <c r="I1371" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="J1371" t="s">
         <v>33</v>
@@ -70600,7 +70603,7 @@
         <v>0</v>
       </c>
       <c r="I1372" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="J1372" t="s">
         <v>30</v>
@@ -70650,7 +70653,7 @@
         <v>0</v>
       </c>
       <c r="I1373" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="J1373" t="s">
         <v>23</v>
@@ -70750,7 +70753,7 @@
         <v>0</v>
       </c>
       <c r="I1375" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="J1375" t="s">
         <v>23</v>
@@ -70800,7 +70803,7 @@
         <v>0</v>
       </c>
       <c r="I1376" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="J1376" t="s">
         <v>33</v>
@@ -70847,10 +70850,10 @@
         <v>0</v>
       </c>
       <c r="I1377" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="J1377" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="K1377" t="b">
         <v>0</v>
@@ -70894,7 +70897,7 @@
         <v>0</v>
       </c>
       <c r="I1378" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="J1378" t="s">
         <v>30</v>
@@ -70944,7 +70947,7 @@
         <v>0</v>
       </c>
       <c r="I1379" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J1379" t="s">
         <v>33</v>
@@ -70991,7 +70994,7 @@
         <v>0</v>
       </c>
       <c r="I1380" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J1380" t="s">
         <v>23</v>
@@ -71088,7 +71091,7 @@
         <v>0</v>
       </c>
       <c r="I1382" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="J1382" t="s">
         <v>40</v>
@@ -71135,7 +71138,7 @@
         <v>0</v>
       </c>
       <c r="I1383" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J1383" t="s">
         <v>30</v>
@@ -71235,7 +71238,7 @@
         <v>0</v>
       </c>
       <c r="I1385" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="J1385" t="s">
         <v>990</v>
@@ -71282,7 +71285,7 @@
         <v>0</v>
       </c>
       <c r="I1386" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="J1386" t="s">
         <v>33</v>
@@ -71376,7 +71379,7 @@
         <v>0</v>
       </c>
       <c r="I1388" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="J1388" t="s">
         <v>23</v>
@@ -71426,7 +71429,7 @@
         <v>0</v>
       </c>
       <c r="I1389" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="J1389" t="s">
         <v>30</v>
@@ -71526,7 +71529,7 @@
         <v>999</v>
       </c>
       <c r="J1391" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="K1391" t="b">
         <v>0</v>
@@ -71620,7 +71623,7 @@
         <v>0</v>
       </c>
       <c r="I1393" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="J1393" t="s">
         <v>23</v>
@@ -71767,7 +71770,7 @@
         <v>0</v>
       </c>
       <c r="I1396" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="J1396" t="s">
         <v>23</v>
@@ -71817,7 +71820,7 @@
         <v>0</v>
       </c>
       <c r="I1397" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="J1397" t="s">
         <v>30</v>
@@ -71867,7 +71870,7 @@
         <v>0</v>
       </c>
       <c r="I1398" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="J1398" t="s">
         <v>23</v>
@@ -71917,7 +71920,7 @@
         <v>0</v>
       </c>
       <c r="I1399" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="J1399" t="s">
         <v>40</v>
@@ -71964,7 +71967,7 @@
         <v>0</v>
       </c>
       <c r="I1400" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="J1400" t="s">
         <v>40</v>
@@ -72011,7 +72014,7 @@
         <v>0</v>
       </c>
       <c r="I1401" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="J1401" t="s">
         <v>40</v>
@@ -72058,7 +72061,7 @@
         <v>0</v>
       </c>
       <c r="I1402" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="J1402" t="s">
         <v>40</v>
@@ -72105,7 +72108,7 @@
         <v>0</v>
       </c>
       <c r="I1403" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="J1403" t="s">
         <v>40</v>
@@ -72152,7 +72155,7 @@
         <v>0</v>
       </c>
       <c r="I1404" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="J1404" t="s">
         <v>40</v>
@@ -72199,7 +72202,7 @@
         <v>0</v>
       </c>
       <c r="I1405" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="J1405" t="s">
         <v>40</v>
@@ -72246,7 +72249,7 @@
         <v>0</v>
       </c>
       <c r="I1406" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="J1406" t="s">
         <v>40</v>
@@ -72293,7 +72296,7 @@
         <v>0</v>
       </c>
       <c r="I1407" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="J1407" t="s">
         <v>40</v>
@@ -72340,7 +72343,7 @@
         <v>0</v>
       </c>
       <c r="I1408" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="J1408" t="s">
         <v>27</v>
@@ -72437,7 +72440,7 @@
         <v>0</v>
       </c>
       <c r="I1410" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="J1410" t="s">
         <v>23</v>
@@ -72487,7 +72490,7 @@
         <v>0</v>
       </c>
       <c r="I1411" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="J1411" t="s">
         <v>33</v>
@@ -72534,7 +72537,7 @@
         <v>0</v>
       </c>
       <c r="I1412" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="J1412" t="s">
         <v>43</v>
@@ -72581,7 +72584,7 @@
         <v>0</v>
       </c>
       <c r="I1413" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="J1413" t="s">
         <v>27</v>
@@ -72678,7 +72681,7 @@
         <v>0</v>
       </c>
       <c r="I1415" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="J1415" t="s">
         <v>30</v>
@@ -72825,7 +72828,7 @@
         <v>0</v>
       </c>
       <c r="I1418" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J1418" t="s">
         <v>23</v>
@@ -72875,7 +72878,7 @@
         <v>0</v>
       </c>
       <c r="I1419" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J1419" t="s">
         <v>33</v>
@@ -72922,7 +72925,7 @@
         <v>0</v>
       </c>
       <c r="I1420" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="J1420" t="s">
         <v>30</v>
@@ -72972,7 +72975,7 @@
         <v>0</v>
       </c>
       <c r="I1421" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="J1421" t="s">
         <v>23</v>
@@ -73069,7 +73072,7 @@
         <v>0</v>
       </c>
       <c r="I1423" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="J1423" t="s">
         <v>30</v>
@@ -73119,7 +73122,7 @@
         <v>0</v>
       </c>
       <c r="I1424" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="J1424" t="s">
         <v>23</v>
@@ -73169,7 +73172,7 @@
         <v>0</v>
       </c>
       <c r="I1425" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="J1425" t="s">
         <v>33</v>
@@ -73216,7 +73219,7 @@
         <v>0</v>
       </c>
       <c r="I1426" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1426" t="s">
         <v>710</v>
@@ -73313,7 +73316,7 @@
         <v>0</v>
       </c>
       <c r="I1428" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="J1428" t="s">
         <v>23</v>
@@ -73363,7 +73366,7 @@
         <v>0</v>
       </c>
       <c r="I1429" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="J1429" t="s">
         <v>30</v>
@@ -73413,10 +73416,10 @@
         <v>0</v>
       </c>
       <c r="I1430" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1430" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="K1430" t="b">
         <v>0</v>
@@ -73460,7 +73463,7 @@
         <v>0</v>
       </c>
       <c r="I1431" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="J1431" t="s">
         <v>30</v>
@@ -73510,7 +73513,7 @@
         <v>0</v>
       </c>
       <c r="I1432" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="J1432" t="s">
         <v>30</v>
@@ -73560,7 +73563,7 @@
         <v>0</v>
       </c>
       <c r="I1433" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="J1433" t="s">
         <v>23</v>
@@ -73657,7 +73660,7 @@
         <v>0</v>
       </c>
       <c r="I1435" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="J1435" t="s">
         <v>40</v>
@@ -73704,7 +73707,7 @@
         <v>0</v>
       </c>
       <c r="I1436" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1436" t="s">
         <v>710</v>
@@ -73801,7 +73804,7 @@
         <v>0</v>
       </c>
       <c r="I1438" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="J1438" t="s">
         <v>23</v>
@@ -73851,7 +73854,7 @@
         <v>0</v>
       </c>
       <c r="I1439" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="J1439" t="s">
         <v>33</v>
@@ -73898,7 +73901,7 @@
         <v>1</v>
       </c>
       <c r="I1440" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="J1440" t="s">
         <v>23</v>
@@ -73948,7 +73951,7 @@
         <v>1</v>
       </c>
       <c r="I1441" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="J1441" t="s">
         <v>30</v>
@@ -73998,7 +74001,7 @@
         <v>0</v>
       </c>
       <c r="I1442" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="J1442" t="s">
         <v>23</v>
@@ -74048,7 +74051,7 @@
         <v>0</v>
       </c>
       <c r="I1443" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="J1443" t="s">
         <v>30</v>
@@ -74098,7 +74101,7 @@
         <v>0</v>
       </c>
       <c r="I1444" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="J1444" t="s">
         <v>33</v>
@@ -74145,10 +74148,10 @@
         <v>0</v>
       </c>
       <c r="I1445" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="J1445" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="K1445" t="b">
         <v>0</v>
@@ -74192,10 +74195,10 @@
         <v>0</v>
       </c>
       <c r="I1446" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="J1446" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K1446" t="b">
         <v>0</v>
@@ -74239,7 +74242,7 @@
         <v>0</v>
       </c>
       <c r="I1447" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1447" t="s">
         <v>710</v>
@@ -74336,7 +74339,7 @@
         <v>0</v>
       </c>
       <c r="I1449" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="J1449" t="s">
         <v>30</v>
@@ -74357,7 +74360,7 @@
         <v>2</v>
       </c>
       <c r="P1449" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1450" spans="1:16" x14ac:dyDescent="0.2">
@@ -74386,7 +74389,7 @@
         <v>0</v>
       </c>
       <c r="I1450" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="J1450" t="s">
         <v>40</v>
@@ -74404,7 +74407,7 @@
         <v>28</v>
       </c>
       <c r="P1450" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1451" spans="1:16" x14ac:dyDescent="0.2">
@@ -74433,7 +74436,7 @@
         <v>0</v>
       </c>
       <c r="I1451" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="J1451" t="s">
         <v>40</v>
@@ -74451,7 +74454,7 @@
         <v>28</v>
       </c>
       <c r="P1451" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1452" spans="1:16" x14ac:dyDescent="0.2">
@@ -74530,7 +74533,7 @@
         <v>0</v>
       </c>
       <c r="I1453" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="J1453" t="s">
         <v>23</v>
@@ -74580,7 +74583,7 @@
         <v>0</v>
       </c>
       <c r="I1454" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="J1454" t="s">
         <v>33</v>
@@ -74627,7 +74630,7 @@
         <v>0</v>
       </c>
       <c r="I1455" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="J1455" t="s">
         <v>299</v>
@@ -74674,7 +74677,7 @@
         <v>0</v>
       </c>
       <c r="I1456" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="J1456" t="s">
         <v>23</v>
@@ -74695,7 +74698,7 @@
         <v>1</v>
       </c>
       <c r="P1456" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1457" spans="1:16" x14ac:dyDescent="0.2">
@@ -74724,7 +74727,7 @@
         <v>0</v>
       </c>
       <c r="I1457" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="J1457" t="s">
         <v>30</v>
@@ -74745,7 +74748,7 @@
         <v>2</v>
       </c>
       <c r="P1457" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1458" spans="1:16" x14ac:dyDescent="0.2">
@@ -74774,7 +74777,7 @@
         <v>0</v>
       </c>
       <c r="I1458" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="J1458" t="s">
         <v>33</v>
@@ -74792,7 +74795,7 @@
         <v>28</v>
       </c>
       <c r="P1458" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1459" spans="1:16" x14ac:dyDescent="0.2">
@@ -74821,7 +74824,7 @@
         <v>0</v>
       </c>
       <c r="I1459" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="J1459" t="s">
         <v>23</v>
@@ -74842,7 +74845,7 @@
         <v>1</v>
       </c>
       <c r="P1459" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1460" spans="1:16" x14ac:dyDescent="0.2">
@@ -74871,7 +74874,7 @@
         <v>0</v>
       </c>
       <c r="I1460" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="J1460" t="s">
         <v>30</v>
@@ -74892,7 +74895,7 @@
         <v>2</v>
       </c>
       <c r="P1460" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1461" spans="1:16" x14ac:dyDescent="0.2">
@@ -74921,7 +74924,7 @@
         <v>0</v>
       </c>
       <c r="I1461" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1461" t="s">
         <v>710</v>
@@ -74939,7 +74942,7 @@
         <v>28</v>
       </c>
       <c r="P1461" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1462" spans="1:16" x14ac:dyDescent="0.2">
@@ -74989,7 +74992,7 @@
         <v>2</v>
       </c>
       <c r="P1462" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1463" spans="1:16" x14ac:dyDescent="0.2">
@@ -75018,7 +75021,7 @@
         <v>0</v>
       </c>
       <c r="I1463" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="J1463" t="s">
         <v>23</v>
@@ -75039,7 +75042,7 @@
         <v>1</v>
       </c>
       <c r="P1463" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1464" spans="1:16" x14ac:dyDescent="0.2">
@@ -75068,7 +75071,7 @@
         <v>0</v>
       </c>
       <c r="I1464" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1464" t="s">
         <v>710</v>
@@ -75086,7 +75089,7 @@
         <v>28</v>
       </c>
       <c r="P1464" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1465" spans="1:16" x14ac:dyDescent="0.2">
@@ -75165,7 +75168,7 @@
         <v>0</v>
       </c>
       <c r="I1466" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="J1466" t="s">
         <v>30</v>
@@ -75215,7 +75218,7 @@
         <v>0</v>
       </c>
       <c r="I1467" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1467" t="s">
         <v>710</v>
@@ -75283,7 +75286,7 @@
         <v>2</v>
       </c>
       <c r="P1468" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1469" spans="1:16" x14ac:dyDescent="0.2">
@@ -75312,7 +75315,7 @@
         <v>0</v>
       </c>
       <c r="I1469" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="J1469" t="s">
         <v>23</v>
@@ -75333,7 +75336,7 @@
         <v>1</v>
       </c>
       <c r="P1469" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1470" spans="1:16" x14ac:dyDescent="0.2">
@@ -75362,7 +75365,7 @@
         <v>0</v>
       </c>
       <c r="I1470" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1470" t="s">
         <v>710</v>
@@ -75380,7 +75383,7 @@
         <v>28</v>
       </c>
       <c r="P1470" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1471" spans="1:16" x14ac:dyDescent="0.2">
@@ -75430,7 +75433,7 @@
         <v>2</v>
       </c>
       <c r="P1471" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1472" spans="1:16" x14ac:dyDescent="0.2">
@@ -75459,7 +75462,7 @@
         <v>0</v>
       </c>
       <c r="I1472" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="J1472" t="s">
         <v>23</v>
@@ -75480,7 +75483,7 @@
         <v>1</v>
       </c>
       <c r="P1472" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1473" spans="1:16" x14ac:dyDescent="0.2">
@@ -75509,7 +75512,7 @@
         <v>0</v>
       </c>
       <c r="I1473" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1473" t="s">
         <v>710</v>
@@ -75527,7 +75530,7 @@
         <v>28</v>
       </c>
       <c r="P1473" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1474" spans="1:16" x14ac:dyDescent="0.2">
@@ -75577,7 +75580,7 @@
         <v>2</v>
       </c>
       <c r="P1474" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1475" spans="1:16" x14ac:dyDescent="0.2">
@@ -75606,7 +75609,7 @@
         <v>0</v>
       </c>
       <c r="I1475" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="J1475" t="s">
         <v>23</v>
@@ -75627,7 +75630,7 @@
         <v>1</v>
       </c>
       <c r="P1475" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1476" spans="1:16" x14ac:dyDescent="0.2">
@@ -75656,7 +75659,7 @@
         <v>0</v>
       </c>
       <c r="I1476" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="J1476" t="s">
         <v>33</v>
@@ -75674,7 +75677,7 @@
         <v>28</v>
       </c>
       <c r="P1476" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1477" spans="1:16" x14ac:dyDescent="0.2">
@@ -75724,7 +75727,7 @@
         <v>2</v>
       </c>
       <c r="P1477" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1478" spans="1:16" x14ac:dyDescent="0.2">
@@ -75753,7 +75756,7 @@
         <v>0</v>
       </c>
       <c r="I1478" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="J1478" t="s">
         <v>23</v>
@@ -75774,7 +75777,7 @@
         <v>1</v>
       </c>
       <c r="P1478" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1479" spans="1:16" x14ac:dyDescent="0.2">
@@ -75803,7 +75806,7 @@
         <v>0</v>
       </c>
       <c r="I1479" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1479" t="s">
         <v>40</v>
@@ -75821,7 +75824,7 @@
         <v>28</v>
       </c>
       <c r="P1479" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1480" spans="1:16" x14ac:dyDescent="0.2">
@@ -75850,7 +75853,7 @@
         <v>0</v>
       </c>
       <c r="I1480" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="J1480" t="s">
         <v>30</v>
@@ -75871,7 +75874,7 @@
         <v>2</v>
       </c>
       <c r="P1480" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1481" spans="1:16" x14ac:dyDescent="0.2">
@@ -75900,7 +75903,7 @@
         <v>0</v>
       </c>
       <c r="I1481" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="J1481" t="s">
         <v>23</v>
@@ -75921,7 +75924,7 @@
         <v>1</v>
       </c>
       <c r="P1481" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1482" spans="1:16" x14ac:dyDescent="0.2">
@@ -75950,7 +75953,7 @@
         <v>0</v>
       </c>
       <c r="I1482" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="J1482" t="s">
         <v>23</v>
@@ -75971,7 +75974,7 @@
         <v>3</v>
       </c>
       <c r="P1482" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1483" spans="1:16" x14ac:dyDescent="0.2">
@@ -76000,7 +76003,7 @@
         <v>0</v>
       </c>
       <c r="I1483" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="J1483" t="s">
         <v>23</v>
@@ -76021,7 +76024,7 @@
         <v>4</v>
       </c>
       <c r="P1483" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1484" spans="1:16" x14ac:dyDescent="0.2">
@@ -76050,7 +76053,7 @@
         <v>0</v>
       </c>
       <c r="I1484" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1484" t="s">
         <v>710</v>
@@ -76068,7 +76071,7 @@
         <v>28</v>
       </c>
       <c r="P1484" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1485" spans="1:16" x14ac:dyDescent="0.2">
@@ -76097,7 +76100,7 @@
         <v>0</v>
       </c>
       <c r="I1485" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="J1485" t="s">
         <v>23</v>
@@ -76118,7 +76121,7 @@
         <v>1</v>
       </c>
       <c r="P1485" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1486" spans="1:16" x14ac:dyDescent="0.2">
@@ -76147,7 +76150,7 @@
         <v>0</v>
       </c>
       <c r="I1486" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="J1486" t="s">
         <v>30</v>
@@ -76168,7 +76171,7 @@
         <v>2</v>
       </c>
       <c r="P1486" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1487" spans="1:16" x14ac:dyDescent="0.2">
@@ -76197,7 +76200,7 @@
         <v>0</v>
       </c>
       <c r="I1487" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1487" t="s">
         <v>710</v>
@@ -76215,7 +76218,7 @@
         <v>28</v>
       </c>
       <c r="P1487" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1488" spans="1:16" x14ac:dyDescent="0.2">
@@ -76244,7 +76247,7 @@
         <v>0</v>
       </c>
       <c r="I1488" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="J1488" t="s">
         <v>30</v>
@@ -76265,7 +76268,7 @@
         <v>2</v>
       </c>
       <c r="P1488" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1489" spans="1:16" x14ac:dyDescent="0.2">
@@ -76294,7 +76297,7 @@
         <v>0</v>
       </c>
       <c r="I1489" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="J1489" t="s">
         <v>23</v>
@@ -76315,7 +76318,7 @@
         <v>1</v>
       </c>
       <c r="P1489" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1490" spans="1:16" x14ac:dyDescent="0.2">
@@ -76344,7 +76347,7 @@
         <v>0</v>
       </c>
       <c r="I1490" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1490" t="s">
         <v>710</v>
@@ -76362,7 +76365,7 @@
         <v>28</v>
       </c>
       <c r="P1490" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1491" spans="1:16" x14ac:dyDescent="0.2">
@@ -76412,7 +76415,7 @@
         <v>1</v>
       </c>
       <c r="P1491" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1492" spans="1:16" x14ac:dyDescent="0.2">
@@ -76441,7 +76444,7 @@
         <v>0</v>
       </c>
       <c r="I1492" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="J1492" t="s">
         <v>30</v>
@@ -76462,7 +76465,7 @@
         <v>2</v>
       </c>
       <c r="P1492" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1493" spans="1:16" x14ac:dyDescent="0.2">
@@ -76491,7 +76494,7 @@
         <v>0</v>
       </c>
       <c r="I1493" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1493" t="s">
         <v>710</v>
@@ -76509,7 +76512,7 @@
         <v>28</v>
       </c>
       <c r="P1493" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1494" spans="1:16" x14ac:dyDescent="0.2">
@@ -76559,7 +76562,7 @@
         <v>1</v>
       </c>
       <c r="P1494" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1495" spans="1:16" x14ac:dyDescent="0.2">
@@ -76588,7 +76591,7 @@
         <v>0</v>
       </c>
       <c r="I1495" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="J1495" t="s">
         <v>30</v>
@@ -76609,7 +76612,7 @@
         <v>2</v>
       </c>
       <c r="P1495" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1496" spans="1:16" x14ac:dyDescent="0.2">
@@ -76638,7 +76641,7 @@
         <v>0</v>
       </c>
       <c r="I1496" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1496" t="s">
         <v>710</v>
@@ -76656,7 +76659,7 @@
         <v>28</v>
       </c>
       <c r="P1496" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1497" spans="1:16" x14ac:dyDescent="0.2">
@@ -76685,7 +76688,7 @@
         <v>0</v>
       </c>
       <c r="I1497" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="J1497" t="s">
         <v>23</v>
@@ -76706,7 +76709,7 @@
         <v>1</v>
       </c>
       <c r="P1497" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1498" spans="1:16" x14ac:dyDescent="0.2">
@@ -76735,7 +76738,7 @@
         <v>0</v>
       </c>
       <c r="I1498" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="J1498" t="s">
         <v>30</v>
@@ -76756,7 +76759,7 @@
         <v>2</v>
       </c>
       <c r="P1498" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1499" spans="1:16" x14ac:dyDescent="0.2">
@@ -76785,7 +76788,7 @@
         <v>0</v>
       </c>
       <c r="I1499" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1499" t="s">
         <v>710</v>
@@ -76803,7 +76806,7 @@
         <v>28</v>
       </c>
       <c r="P1499" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1500" spans="1:16" x14ac:dyDescent="0.2">
@@ -76832,7 +76835,7 @@
         <v>0</v>
       </c>
       <c r="I1500" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="J1500" t="s">
         <v>30</v>
@@ -76853,7 +76856,7 @@
         <v>2</v>
       </c>
       <c r="P1500" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1501" spans="1:16" x14ac:dyDescent="0.2">
@@ -76882,7 +76885,7 @@
         <v>0</v>
       </c>
       <c r="I1501" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="J1501" t="s">
         <v>23</v>
@@ -76903,7 +76906,7 @@
         <v>1</v>
       </c>
       <c r="P1501" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1502" spans="1:16" x14ac:dyDescent="0.2">
@@ -76932,7 +76935,7 @@
         <v>0</v>
       </c>
       <c r="I1502" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1502" t="s">
         <v>710</v>
@@ -76950,7 +76953,7 @@
         <v>28</v>
       </c>
       <c r="P1502" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1503" spans="1:16" x14ac:dyDescent="0.2">
@@ -77000,7 +77003,7 @@
         <v>2</v>
       </c>
       <c r="P1503" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1504" spans="1:16" x14ac:dyDescent="0.2">
@@ -77029,7 +77032,7 @@
         <v>0</v>
       </c>
       <c r="I1504" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="J1504" t="s">
         <v>23</v>
@@ -77050,7 +77053,7 @@
         <v>1</v>
       </c>
       <c r="P1504" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1505" spans="1:16" x14ac:dyDescent="0.2">
@@ -77079,7 +77082,7 @@
         <v>0</v>
       </c>
       <c r="I1505" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1505" t="s">
         <v>710</v>
@@ -77097,7 +77100,7 @@
         <v>28</v>
       </c>
       <c r="P1505" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1506" spans="1:16" x14ac:dyDescent="0.2">
@@ -77126,7 +77129,7 @@
         <v>0</v>
       </c>
       <c r="I1506" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="J1506" t="s">
         <v>30</v>
@@ -77147,7 +77150,7 @@
         <v>2</v>
       </c>
       <c r="P1506" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1507" spans="1:16" x14ac:dyDescent="0.2">
@@ -77176,7 +77179,7 @@
         <v>0</v>
       </c>
       <c r="I1507" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="J1507" t="s">
         <v>23</v>
@@ -77197,7 +77200,7 @@
         <v>1</v>
       </c>
       <c r="P1507" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1508" spans="1:16" x14ac:dyDescent="0.2">
@@ -77226,7 +77229,7 @@
         <v>0</v>
       </c>
       <c r="I1508" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1508" t="s">
         <v>710</v>
@@ -77244,7 +77247,7 @@
         <v>28</v>
       </c>
       <c r="P1508" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1509" spans="1:16" x14ac:dyDescent="0.2">
@@ -77294,7 +77297,7 @@
         <v>2</v>
       </c>
       <c r="P1509" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1510" spans="1:16" x14ac:dyDescent="0.2">
@@ -77323,7 +77326,7 @@
         <v>0</v>
       </c>
       <c r="I1510" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="J1510" t="s">
         <v>23</v>
@@ -77344,7 +77347,7 @@
         <v>1</v>
       </c>
       <c r="P1510" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1511" spans="1:16" x14ac:dyDescent="0.2">
@@ -77373,7 +77376,7 @@
         <v>0</v>
       </c>
       <c r="I1511" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1511" t="s">
         <v>710</v>
@@ -77391,7 +77394,7 @@
         <v>28</v>
       </c>
       <c r="P1511" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1512" spans="1:16" x14ac:dyDescent="0.2">
@@ -77470,7 +77473,7 @@
         <v>0</v>
       </c>
       <c r="I1513" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="J1513" t="s">
         <v>30</v>
@@ -77520,7 +77523,7 @@
         <v>0</v>
       </c>
       <c r="I1514" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1514" t="s">
         <v>710</v>
@@ -77567,7 +77570,7 @@
         <v>0</v>
       </c>
       <c r="I1515" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="J1515" t="s">
         <v>23</v>
@@ -77588,7 +77591,7 @@
         <v>1</v>
       </c>
       <c r="P1515" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1516" spans="1:16" x14ac:dyDescent="0.2">
@@ -77617,7 +77620,7 @@
         <v>0</v>
       </c>
       <c r="I1516" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="J1516" t="s">
         <v>30</v>
@@ -77638,7 +77641,7 @@
         <v>2</v>
       </c>
       <c r="P1516" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1517" spans="1:16" x14ac:dyDescent="0.2">
@@ -77667,7 +77670,7 @@
         <v>0</v>
       </c>
       <c r="I1517" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1517" t="s">
         <v>710</v>
@@ -77685,7 +77688,7 @@
         <v>28</v>
       </c>
       <c r="P1517" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1518" spans="1:16" x14ac:dyDescent="0.2">
@@ -77735,7 +77738,7 @@
         <v>2</v>
       </c>
       <c r="P1518" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1519" spans="1:16" x14ac:dyDescent="0.2">
@@ -77764,7 +77767,7 @@
         <v>0</v>
       </c>
       <c r="I1519" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="J1519" t="s">
         <v>23</v>
@@ -77785,7 +77788,7 @@
         <v>1</v>
       </c>
       <c r="P1519" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1520" spans="1:16" x14ac:dyDescent="0.2">
@@ -77814,7 +77817,7 @@
         <v>0</v>
       </c>
       <c r="I1520" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1520" t="s">
         <v>710</v>
@@ -77832,7 +77835,7 @@
         <v>28</v>
       </c>
       <c r="P1520" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1521" spans="1:16" x14ac:dyDescent="0.2">
@@ -77882,7 +77885,7 @@
         <v>2</v>
       </c>
       <c r="P1521" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1522" spans="1:16" x14ac:dyDescent="0.2">
@@ -77911,7 +77914,7 @@
         <v>0</v>
       </c>
       <c r="I1522" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="J1522" t="s">
         <v>23</v>
@@ -77932,7 +77935,7 @@
         <v>1</v>
       </c>
       <c r="P1522" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1523" spans="1:16" x14ac:dyDescent="0.2">
@@ -77961,7 +77964,7 @@
         <v>0</v>
       </c>
       <c r="I1523" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="J1523" t="s">
         <v>33</v>
@@ -77979,7 +77982,7 @@
         <v>28</v>
       </c>
       <c r="P1523" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1524" spans="1:16" x14ac:dyDescent="0.2">
@@ -78029,7 +78032,7 @@
         <v>2</v>
       </c>
       <c r="P1524" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1525" spans="1:16" x14ac:dyDescent="0.2">
@@ -78058,7 +78061,7 @@
         <v>0</v>
       </c>
       <c r="I1525" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="J1525" t="s">
         <v>23</v>
@@ -78079,7 +78082,7 @@
         <v>3</v>
       </c>
       <c r="P1525" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1526" spans="1:16" x14ac:dyDescent="0.2">
@@ -78108,7 +78111,7 @@
         <v>0</v>
       </c>
       <c r="I1526" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="J1526" t="s">
         <v>33</v>
@@ -78129,7 +78132,7 @@
         <v>4</v>
       </c>
       <c r="P1526" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1527" spans="1:16" x14ac:dyDescent="0.2">
@@ -78158,10 +78161,10 @@
         <v>0</v>
       </c>
       <c r="I1527" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1527" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="K1527" t="b">
         <v>1</v>
@@ -78176,7 +78179,7 @@
         <v>28</v>
       </c>
       <c r="P1527" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1528" spans="1:16" x14ac:dyDescent="0.2">
@@ -78205,10 +78208,10 @@
         <v>0</v>
       </c>
       <c r="I1528" t="s">
+        <v>1337</v>
+      </c>
+      <c r="J1528" t="s">
         <v>1338</v>
-      </c>
-      <c r="J1528" t="s">
-        <v>1339</v>
       </c>
       <c r="K1528" t="b">
         <v>0</v>
@@ -78226,7 +78229,7 @@
         <v>1</v>
       </c>
       <c r="P1528" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1529" spans="1:16" x14ac:dyDescent="0.2">
@@ -78255,7 +78258,7 @@
         <v>0</v>
       </c>
       <c r="I1529" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="J1529" t="s">
         <v>23</v>
@@ -78276,7 +78279,7 @@
         <v>1</v>
       </c>
       <c r="P1529" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1530" spans="1:16" x14ac:dyDescent="0.2">
@@ -78305,7 +78308,7 @@
         <v>0</v>
       </c>
       <c r="I1530" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="J1530" t="s">
         <v>30</v>
@@ -78326,7 +78329,7 @@
         <v>2</v>
       </c>
       <c r="P1530" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1531" spans="1:16" x14ac:dyDescent="0.2">
@@ -78355,7 +78358,7 @@
         <v>0</v>
       </c>
       <c r="I1531" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="J1531" t="s">
         <v>710</v>
@@ -78373,7 +78376,7 @@
         <v>28</v>
       </c>
       <c r="P1531" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1532" spans="1:16" x14ac:dyDescent="0.2">
@@ -78423,7 +78426,7 @@
         <v>1</v>
       </c>
       <c r="P1532" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1533" spans="1:16" x14ac:dyDescent="0.2">
@@ -78452,7 +78455,7 @@
         <v>0</v>
       </c>
       <c r="I1533" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="J1533" t="s">
         <v>30</v>
@@ -78473,7 +78476,7 @@
         <v>2</v>
       </c>
       <c r="P1533" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1534" spans="1:16" x14ac:dyDescent="0.2">
@@ -78502,7 +78505,7 @@
         <v>0</v>
       </c>
       <c r="I1534" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1534" t="s">
         <v>710</v>
@@ -78520,7 +78523,7 @@
         <v>28</v>
       </c>
       <c r="P1534" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1535" spans="1:16" x14ac:dyDescent="0.2">
@@ -78549,7 +78552,7 @@
         <v>0</v>
       </c>
       <c r="I1535" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="J1535" t="s">
         <v>30</v>
@@ -78570,7 +78573,7 @@
         <v>2</v>
       </c>
       <c r="P1535" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1536" spans="1:16" x14ac:dyDescent="0.2">
@@ -78599,7 +78602,7 @@
         <v>0</v>
       </c>
       <c r="I1536" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="J1536" t="s">
         <v>23</v>
@@ -78620,7 +78623,7 @@
         <v>1</v>
       </c>
       <c r="P1536" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1537" spans="1:16" x14ac:dyDescent="0.2">
@@ -78649,10 +78652,10 @@
         <v>0</v>
       </c>
       <c r="I1537" t="s">
+        <v>1348</v>
+      </c>
+      <c r="J1537" t="s">
         <v>1349</v>
-      </c>
-      <c r="J1537" t="s">
-        <v>1350</v>
       </c>
       <c r="K1537" t="b">
         <v>0</v>
@@ -78667,7 +78670,7 @@
         <v>28</v>
       </c>
       <c r="P1537" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1538" spans="1:16" x14ac:dyDescent="0.2">
@@ -78696,7 +78699,7 @@
         <v>0</v>
       </c>
       <c r="I1538" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="J1538" t="s">
         <v>710</v>
@@ -78714,7 +78717,7 @@
         <v>28</v>
       </c>
       <c r="P1538" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>